<commit_message>
Updated sentiment analysis code to include ground truth labeling and classifier results
</commit_message>
<xml_diff>
--- a/SentimentAnalysis/sentment.xlsx
+++ b/SentimentAnalysis/sentment.xlsx
@@ -693,7 +693,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.208695652173913</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -704,7 +704,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.2307692307692308</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -715,7 +715,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.2666666666666667</v>
+        <v>-1.382608695652174</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -726,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.1333333333333333</v>
+        <v>0.02678571428571428</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -737,7 +737,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.7333333333333333</v>
+        <v>0.1142857142857143</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -748,7 +748,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.2</v>
+        <v>-0.7631578947368421</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -759,7 +759,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.6</v>
+        <v>-0.4869565217391305</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -770,7 +770,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.4666666666666667</v>
+        <v>-0.6605504587155964</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -781,7 +781,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>0.06666666666666667</v>
+        <v>-0.01739130434782609</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -792,7 +792,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.7333333333333333</v>
+        <v>-0.6153846153846154</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -803,7 +803,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.8</v>
+        <v>-0.09565217391304348</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -814,7 +814,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.3333333333333333</v>
+        <v>-0.2123893805309734</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -825,7 +825,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1333333333333333</v>
+        <v>-0.4260869565217391</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -836,7 +836,7 @@
         <v>15</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.4666666666666667</v>
+        <v>-0.05217391304347826</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -847,7 +847,7 @@
         <v>16</v>
       </c>
       <c r="C16" t="n">
-        <v>0.06666666666666667</v>
+        <v>-0.1130434782608696</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -858,7 +858,7 @@
         <v>17</v>
       </c>
       <c r="C17" t="n">
-        <v>-2.266666666666667</v>
+        <v>-1.704347826086956</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -869,7 +869,7 @@
         <v>18</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6</v>
+        <v>-2.017391304347826</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -880,7 +880,7 @@
         <v>19</v>
       </c>
       <c r="C19" t="n">
-        <v>1.8</v>
+        <v>1.150442477876106</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -891,7 +891,7 @@
         <v>20</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.9333333333333333</v>
+        <v>-0.6260869565217392</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -902,7 +902,7 @@
         <v>21</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.2666666666666667</v>
+        <v>0.6086956521739131</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -913,7 +913,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="n">
-        <v>0.2666666666666667</v>
+        <v>-0.4774774774774775</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -924,7 +924,7 @@
         <v>23</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.7333333333333333</v>
+        <v>0.4260869565217391</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -935,7 +935,7 @@
         <v>24</v>
       </c>
       <c r="C24" t="n">
-        <v>0.06666666666666667</v>
+        <v>-0.02631578947368421</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -946,7 +946,7 @@
         <v>25</v>
       </c>
       <c r="C25" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.2347826086956522</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -957,7 +957,7 @@
         <v>26</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.2666666666666667</v>
+        <v>0.3304347826086956</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -968,7 +968,7 @@
         <v>27</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.1333333333333333</v>
+        <v>0.03636363636363636</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -979,7 +979,7 @@
         <v>28</v>
       </c>
       <c r="C28" t="n">
-        <v>0.2</v>
+        <v>0.3035714285714285</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -990,7 +990,7 @@
         <v>29</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.06666666666666667</v>
+        <v>-0.6491228070175439</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1001,7 +1001,7 @@
         <v>30</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.8</v>
+        <v>-0.1923076923076923</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1012,7 +1012,7 @@
         <v>31</v>
       </c>
       <c r="C31" t="n">
-        <v>0.2</v>
+        <v>-0.3482142857142857</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1023,7 +1023,7 @@
         <v>32</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.2</v>
+        <v>-0.4470588235294118</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1034,7 +1034,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="n">
-        <v>0.06666666666666667</v>
+        <v>-0.2260869565217391</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1045,7 +1045,7 @@
         <v>34</v>
       </c>
       <c r="C34" t="n">
-        <v>0.1333333333333333</v>
+        <v>0.04347826086956522</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1056,7 +1056,7 @@
         <v>35</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.6666666666666666</v>
+        <v>-1.147826086956522</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1067,7 +1067,7 @@
         <v>36</v>
       </c>
       <c r="C36" t="n">
-        <v>-1.6</v>
+        <v>-0.7478260869565218</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1078,7 +1078,7 @@
         <v>37</v>
       </c>
       <c r="C37" t="n">
-        <v>-2.2</v>
+        <v>-1.069565217391304</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1089,7 +1089,7 @@
         <v>38</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.4</v>
+        <v>0.3130434782608696</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1100,7 +1100,7 @@
         <v>39</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.06666666666666667</v>
+        <v>0.616822429906542</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1111,7 +1111,7 @@
         <v>40</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.1333333333333333</v>
+        <v>0.4956521739130435</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1122,7 +1122,7 @@
         <v>41</v>
       </c>
       <c r="C41" t="n">
-        <v>0.5333333333333333</v>
+        <v>1.626086956521739</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1133,7 +1133,7 @@
         <v>42</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.9333333333333333</v>
+        <v>-0.7731958762886598</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1144,7 +1144,7 @@
         <v>43</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.6</v>
+        <v>-0.4260869565217391</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1155,7 +1155,7 @@
         <v>44</v>
       </c>
       <c r="C44" t="n">
-        <v>0.6</v>
+        <v>0.06086956521739131</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1166,7 +1166,7 @@
         <v>45</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.3333333333333333</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1177,7 +1177,7 @@
         <v>46</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.9333333333333333</v>
+        <v>-0.6695652173913044</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1188,7 +1188,7 @@
         <v>47</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.3333333333333333</v>
+        <v>-0.4084507042253521</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1199,7 +1199,7 @@
         <v>48</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.1333333333333333</v>
+        <v>-0.2589285714285715</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1210,7 +1210,7 @@
         <v>49</v>
       </c>
       <c r="C49" t="n">
-        <v>0.1333333333333333</v>
+        <v>0.5391304347826087</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1221,7 +1221,7 @@
         <v>50</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.06666666666666667</v>
+        <v>-0.7787610619469026</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1232,7 +1232,7 @@
         <v>51</v>
       </c>
       <c r="C51" t="n">
-        <v>1.2</v>
+        <v>0.208695652173913</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1243,7 +1243,7 @@
         <v>52</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.6666666666666666</v>
+        <v>0.1826086956521739</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1254,7 +1254,7 @@
         <v>53</v>
       </c>
       <c r="C53" t="n">
-        <v>0.1333333333333333</v>
+        <v>-0.4608695652173913</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1265,7 +1265,7 @@
         <v>54</v>
       </c>
       <c r="C54" t="n">
-        <v>0.3333333333333333</v>
+        <v>-0.7217391304347827</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1276,7 +1276,7 @@
         <v>55</v>
       </c>
       <c r="C55" t="n">
-        <v>-1.2</v>
+        <v>-0.8956521739130435</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1287,7 +1287,7 @@
         <v>56</v>
       </c>
       <c r="C56" t="n">
-        <v>0.2</v>
+        <v>-0.2173913043478261</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1298,7 +1298,7 @@
         <v>57</v>
       </c>
       <c r="C57" t="n">
-        <v>1.8</v>
+        <v>2.356521739130435</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1309,7 +1309,7 @@
         <v>58</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.7333333333333333</v>
+        <v>-0.9587628865979382</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1320,7 +1320,7 @@
         <v>59</v>
       </c>
       <c r="C59" t="n">
-        <v>0.2</v>
+        <v>-0.1130434782608696</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1331,7 +1331,7 @@
         <v>60</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.2</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1342,7 +1342,7 @@
         <v>61</v>
       </c>
       <c r="C61" t="n">
-        <v>0.1333333333333333</v>
+        <v>-0.23</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1353,7 +1353,7 @@
         <v>62</v>
       </c>
       <c r="C62" t="n">
-        <v>0.1333333333333333</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1364,7 +1364,7 @@
         <v>63</v>
       </c>
       <c r="C63" t="n">
-        <v>-0.9333333333333333</v>
+        <v>-0.7816091954022989</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1375,7 +1375,7 @@
         <v>64</v>
       </c>
       <c r="C64" t="n">
-        <v>-1.066666666666667</v>
+        <v>-1.31</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1386,7 +1386,7 @@
         <v>65</v>
       </c>
       <c r="C65" t="n">
-        <v>1</v>
+        <v>-0.35</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1397,7 +1397,7 @@
         <v>66</v>
       </c>
       <c r="C66" t="n">
-        <v>-0.6</v>
+        <v>-1.145833333333333</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1408,7 +1408,7 @@
         <v>67</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.3333333333333333</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1419,7 +1419,7 @@
         <v>68</v>
       </c>
       <c r="C68" t="n">
-        <v>0.5333333333333333</v>
+        <v>-0.4393939393939394</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1430,7 +1430,7 @@
         <v>69</v>
       </c>
       <c r="C69" t="n">
-        <v>0.1333333333333333</v>
+        <v>-0.3292682926829268</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1441,7 +1441,7 @@
         <v>70</v>
       </c>
       <c r="C70" t="n">
-        <v>1.733333333333333</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1452,7 +1452,7 @@
         <v>71</v>
       </c>
       <c r="C71" t="n">
-        <v>-0.2</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1463,7 +1463,7 @@
         <v>72</v>
       </c>
       <c r="C72" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1474,7 +1474,7 @@
         <v>73</v>
       </c>
       <c r="C73" t="n">
-        <v>0.06666666666666667</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1485,7 +1485,7 @@
         <v>74</v>
       </c>
       <c r="C74" t="n">
-        <v>-0.2666666666666667</v>
+        <v>-0.22</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1496,7 +1496,7 @@
         <v>75</v>
       </c>
       <c r="C75" t="n">
-        <v>-1.533333333333333</v>
+        <v>-0.95</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1507,7 +1507,7 @@
         <v>76</v>
       </c>
       <c r="C76" t="n">
-        <v>-0.2</v>
+        <v>-2.66</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1518,7 +1518,7 @@
         <v>77</v>
       </c>
       <c r="C77" t="n">
-        <v>0.1333333333333333</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1529,7 +1529,7 @@
         <v>78</v>
       </c>
       <c r="C78" t="n">
-        <v>-0.4</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1540,7 +1540,7 @@
         <v>79</v>
       </c>
       <c r="C79" t="n">
-        <v>-1</v>
+        <v>-0.32</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1551,7 +1551,7 @@
         <v>80</v>
       </c>
       <c r="C80" t="n">
-        <v>-0.5333333333333333</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1562,7 +1562,7 @@
         <v>81</v>
       </c>
       <c r="C81" t="n">
-        <v>1.4</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1573,7 +1573,7 @@
         <v>82</v>
       </c>
       <c r="C82" t="n">
-        <v>-2.4</v>
+        <v>-1.16</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1584,7 +1584,7 @@
         <v>83</v>
       </c>
       <c r="C83" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.4230769230769231</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1595,7 +1595,7 @@
         <v>84</v>
       </c>
       <c r="C84" t="n">
-        <v>0.6</v>
+        <v>-2.857142857142857</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1606,7 +1606,7 @@
         <v>85</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1617,7 +1617,7 @@
         <v>86</v>
       </c>
       <c r="C86" t="n">
-        <v>-0.2</v>
+        <v>-0.18</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1628,7 +1628,7 @@
         <v>87</v>
       </c>
       <c r="C87" t="n">
-        <v>0.4</v>
+        <v>-0.1515151515151515</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1639,7 +1639,7 @@
         <v>88</v>
       </c>
       <c r="C88" t="n">
-        <v>0.1333333333333333</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1650,7 +1650,7 @@
         <v>89</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1661,7 +1661,7 @@
         <v>90</v>
       </c>
       <c r="C90" t="n">
-        <v>2</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1672,7 +1672,7 @@
         <v>91</v>
       </c>
       <c r="C91" t="n">
-        <v>1</v>
+        <v>-0.8100000000000001</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1683,7 +1683,7 @@
         <v>92</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.8</v>
+        <v>-0.27</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1694,7 +1694,7 @@
         <v>93</v>
       </c>
       <c r="C93" t="n">
-        <v>-0.06666666666666667</v>
+        <v>-1.14</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1705,7 +1705,7 @@
         <v>94</v>
       </c>
       <c r="C94" t="n">
-        <v>-0.1333333333333333</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1716,7 +1716,7 @@
         <v>95</v>
       </c>
       <c r="C95" t="n">
-        <v>-1</v>
+        <v>-1.119565217391304</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1727,7 +1727,7 @@
         <v>96</v>
       </c>
       <c r="C96" t="n">
-        <v>-0.1333333333333333</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1738,7 +1738,7 @@
         <v>97</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.6</v>
+        <v>-0.99</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1749,7 +1749,7 @@
         <v>98</v>
       </c>
       <c r="C98" t="n">
-        <v>-0.3333333333333333</v>
+        <v>-0.52</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1760,7 +1760,7 @@
         <v>99</v>
       </c>
       <c r="C99" t="n">
-        <v>-0.06666666666666667</v>
+        <v>0.1263157894736842</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1771,7 +1771,7 @@
         <v>100</v>
       </c>
       <c r="C100" t="n">
-        <v>-0.5333333333333333</v>
+        <v>-0.43</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1782,7 +1782,7 @@
         <v>101</v>
       </c>
       <c r="C101" t="n">
-        <v>-0.5333333333333333</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>